<commit_message>
MOD arreglar fallo data stock
</commit_message>
<xml_diff>
--- a/data/inventory_data_stock.xlsx
+++ b/data/inventory_data_stock.xlsx
@@ -526,7 +526,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B2" t="n">
         <v>114230822</v>
@@ -568,7 +568,7 @@
         <v>-45</v>
       </c>
       <c r="O2" t="n">
-        <v>-15</v>
+        <v>49</v>
       </c>
       <c r="P2" t="n">
         <v>66500</v>
@@ -577,12 +577,12 @@
         <v>2292.96</v>
       </c>
       <c r="R2" t="n">
-        <v>0.0344806015037594</v>
+        <v>0.034480601503759</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B3" t="n">
         <v>115030252</v>
@@ -624,7 +624,7 @@
         <v>26</v>
       </c>
       <c r="O3" t="n">
-        <v>-50</v>
+        <v>120</v>
       </c>
       <c r="P3" t="n">
         <v>23000</v>
@@ -638,7 +638,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="B4" t="n">
         <v>115070602</v>
@@ -694,7 +694,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="B5" t="n">
         <v>115130209</v>
@@ -750,7 +750,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="B6" t="n">
         <v>115170581</v>
@@ -806,7 +806,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="B7" t="n">
         <v>116211401</v>
@@ -862,7 +862,7 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="B8" t="n">
         <v>116490250</v>
@@ -906,7 +906,7 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="B9" t="n">
         <v>116490259</v>
@@ -962,7 +962,7 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="B10" t="n">
         <v>118030902</v>
@@ -1018,7 +1018,7 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="B11" t="n">
         <v>118030904</v>
@@ -1074,7 +1074,7 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="B12" t="n">
         <v>118130103</v>
@@ -1130,7 +1130,7 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="B13" t="n">
         <v>133062220</v>
@@ -1172,7 +1172,7 @@
         <v>9</v>
       </c>
       <c r="O13" t="n">
-        <v>-21</v>
+        <v>103</v>
       </c>
       <c r="P13" t="n">
         <v>144000</v>
@@ -1186,7 +1186,7 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>64</v>
+        <v>12</v>
       </c>
       <c r="B14" t="n">
         <v>133062421</v>
@@ -1242,7 +1242,7 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>69</v>
+        <v>13</v>
       </c>
       <c r="B15" t="n">
         <v>133065201</v>
@@ -1298,7 +1298,7 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="B16" t="n">
         <v>133065207</v>
@@ -1340,7 +1340,7 @@
         <v>-37</v>
       </c>
       <c r="O16" t="n">
-        <v>-27</v>
+        <v>57</v>
       </c>
       <c r="P16" t="n">
         <v>30600</v>
@@ -1354,7 +1354,7 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>74</v>
+        <v>15</v>
       </c>
       <c r="B17" t="n">
         <v>133065216</v>
@@ -1410,7 +1410,7 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>76</v>
+        <v>16</v>
       </c>
       <c r="B18" t="n">
         <v>133065270</v>
@@ -1466,7 +1466,7 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="B19" t="n">
         <v>133065271</v>
@@ -1522,7 +1522,7 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>80</v>
+        <v>18</v>
       </c>
       <c r="B20" t="n">
         <v>133066003</v>
@@ -1578,7 +1578,7 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>81</v>
+        <v>19</v>
       </c>
       <c r="B21" t="n">
         <v>133066421</v>
@@ -1634,7 +1634,7 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>83</v>
+        <v>20</v>
       </c>
       <c r="B22" t="n">
         <v>133066424</v>
@@ -1690,7 +1690,7 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>85</v>
+        <v>21</v>
       </c>
       <c r="B23" t="n">
         <v>133066428</v>
@@ -1746,7 +1746,7 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>87</v>
+        <v>22</v>
       </c>
       <c r="B24" t="n">
         <v>133066431</v>
@@ -1802,7 +1802,7 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>90</v>
+        <v>23</v>
       </c>
       <c r="B25" t="n">
         <v>133066450</v>
@@ -1858,7 +1858,7 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>91</v>
+        <v>24</v>
       </c>
       <c r="B26" t="n">
         <v>133066451</v>
@@ -1900,7 +1900,7 @@
         <v>-61</v>
       </c>
       <c r="O26" t="n">
-        <v>-3</v>
+        <v>33</v>
       </c>
       <c r="P26" t="n">
         <v>288000</v>
@@ -1914,7 +1914,7 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>92</v>
+        <v>25</v>
       </c>
       <c r="B27" t="n">
         <v>133066452</v>
@@ -1970,7 +1970,7 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>94</v>
+        <v>26</v>
       </c>
       <c r="B28" t="n">
         <v>133066461</v>
@@ -2026,7 +2026,7 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>99</v>
+        <v>27</v>
       </c>
       <c r="B29" t="n">
         <v>133066531</v>
@@ -2082,7 +2082,7 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>100</v>
+        <v>28</v>
       </c>
       <c r="B30" t="n">
         <v>133066532</v>
@@ -2128,7 +2128,7 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>105</v>
+        <v>29</v>
       </c>
       <c r="B31" t="n">
         <v>133066550</v>
@@ -2184,7 +2184,7 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>110</v>
+        <v>30</v>
       </c>
       <c r="B32" t="n">
         <v>133066701</v>
@@ -2230,7 +2230,7 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>114</v>
+        <v>31</v>
       </c>
       <c r="B33" t="n">
         <v>133067502</v>
@@ -2286,7 +2286,7 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>116</v>
+        <v>32</v>
       </c>
       <c r="B34" t="n">
         <v>133067532</v>
@@ -2342,7 +2342,7 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>117</v>
+        <v>33</v>
       </c>
       <c r="B35" t="n">
         <v>133068500</v>
@@ -2398,7 +2398,7 @@
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>118</v>
+        <v>34</v>
       </c>
       <c r="B36" t="n">
         <v>133068501</v>
@@ -2454,7 +2454,7 @@
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>124</v>
+        <v>35</v>
       </c>
       <c r="B37" t="n">
         <v>133100502</v>
@@ -2510,7 +2510,7 @@
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>127</v>
+        <v>36</v>
       </c>
       <c r="B38" t="n">
         <v>133121045</v>
@@ -2566,7 +2566,7 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>129</v>
+        <v>37</v>
       </c>
       <c r="B39" t="n">
         <v>133160110</v>
@@ -2608,7 +2608,7 @@
         <v>-58</v>
       </c>
       <c r="O39" t="n">
-        <v>-6</v>
+        <v>36</v>
       </c>
       <c r="P39" t="n">
         <v>726000</v>
@@ -2622,7 +2622,7 @@
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>132</v>
+        <v>38</v>
       </c>
       <c r="B40" t="n">
         <v>133200405</v>
@@ -2678,7 +2678,7 @@
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>137</v>
+        <v>39</v>
       </c>
       <c r="B41" t="n">
         <v>134055103</v>
@@ -2734,7 +2734,7 @@
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>138</v>
+        <v>40</v>
       </c>
       <c r="B42" t="n">
         <v>134059411</v>
@@ -2790,7 +2790,7 @@
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>139</v>
+        <v>41</v>
       </c>
       <c r="B43" t="n">
         <v>134060101</v>
@@ -2834,7 +2834,7 @@
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>141</v>
+        <v>42</v>
       </c>
       <c r="B44" t="n">
         <v>134060502</v>
@@ -2876,7 +2876,7 @@
         <v>-57</v>
       </c>
       <c r="O44" t="n">
-        <v>-3</v>
+        <v>37</v>
       </c>
       <c r="P44" t="n">
         <v>150000</v>
@@ -2890,7 +2890,7 @@
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>142</v>
+        <v>43</v>
       </c>
       <c r="B45" t="n">
         <v>134060503</v>
@@ -2946,7 +2946,7 @@
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>147</v>
+        <v>44</v>
       </c>
       <c r="B46" t="n">
         <v>134140101</v>
@@ -3002,7 +3002,7 @@
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>155</v>
+        <v>45</v>
       </c>
       <c r="B47" t="n">
         <v>134320133</v>
@@ -3058,7 +3058,7 @@
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>158</v>
+        <v>46</v>
       </c>
       <c r="B48" t="n">
         <v>134320136</v>
@@ -3114,7 +3114,7 @@
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>166</v>
+        <v>47</v>
       </c>
       <c r="B49" t="n">
         <v>134321006</v>
@@ -3156,7 +3156,7 @@
         <v>-52</v>
       </c>
       <c r="O49" t="n">
-        <v>-8</v>
+        <v>42</v>
       </c>
       <c r="P49" t="n">
         <v>243100</v>
@@ -3170,7 +3170,7 @@
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>171</v>
+        <v>48</v>
       </c>
       <c r="B50" t="n">
         <v>135030110</v>
@@ -3226,7 +3226,7 @@
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>172</v>
+        <v>49</v>
       </c>
       <c r="B51" t="n">
         <v>135030111</v>
@@ -3282,7 +3282,7 @@
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>174</v>
+        <v>50</v>
       </c>
       <c r="B52" t="n">
         <v>135030114</v>
@@ -3324,7 +3324,7 @@
         <v>-61</v>
       </c>
       <c r="O52" t="n">
-        <v>-3</v>
+        <v>33</v>
       </c>
       <c r="P52" t="n">
         <v>249050</v>
@@ -3338,7 +3338,7 @@
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>175</v>
+        <v>51</v>
       </c>
       <c r="B53" t="n">
         <v>135030117</v>
@@ -3394,7 +3394,7 @@
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>180</v>
+        <v>52</v>
       </c>
       <c r="B54" t="n">
         <v>135030207</v>
@@ -3450,7 +3450,7 @@
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>183</v>
+        <v>53</v>
       </c>
       <c r="B55" t="n">
         <v>135030210</v>
@@ -3506,7 +3506,7 @@
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>187</v>
+        <v>54</v>
       </c>
       <c r="B56" t="n">
         <v>135060113</v>
@@ -3562,7 +3562,7 @@
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>196</v>
+        <v>55</v>
       </c>
       <c r="B57" t="n">
         <v>135060909</v>
@@ -3618,7 +3618,7 @@
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>197</v>
+        <v>56</v>
       </c>
       <c r="B58" t="n">
         <v>135060910</v>
@@ -3660,7 +3660,7 @@
         <v>65</v>
       </c>
       <c r="O58" t="n">
-        <v>-10</v>
+        <v>159</v>
       </c>
       <c r="P58" t="n">
         <v>106250</v>
@@ -3674,7 +3674,7 @@
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>200</v>
+        <v>57</v>
       </c>
       <c r="B59" t="n">
         <v>135061014</v>
@@ -3716,7 +3716,7 @@
         <v>-26</v>
       </c>
       <c r="O59" t="n">
-        <v>-34</v>
+        <v>68</v>
       </c>
       <c r="P59" t="n">
         <v>51000</v>
@@ -3730,7 +3730,7 @@
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>201</v>
+        <v>58</v>
       </c>
       <c r="B60" t="n">
         <v>135061015</v>
@@ -3786,7 +3786,7 @@
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
-        <v>202</v>
+        <v>59</v>
       </c>
       <c r="B61" t="n">
         <v>135061019</v>
@@ -3828,7 +3828,7 @@
         <v>-16</v>
       </c>
       <c r="O61" t="n">
-        <v>-44</v>
+        <v>78</v>
       </c>
       <c r="P61" t="n">
         <v>170000</v>
@@ -3842,7 +3842,7 @@
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>212</v>
+        <v>60</v>
       </c>
       <c r="B62" t="n">
         <v>135062142</v>
@@ -3884,7 +3884,7 @@
         <v>-61</v>
       </c>
       <c r="O62" t="n">
-        <v>-3</v>
+        <v>33</v>
       </c>
       <c r="P62" t="n">
         <v>2492200</v>
@@ -3898,7 +3898,7 @@
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>213</v>
+        <v>61</v>
       </c>
       <c r="B63" t="n">
         <v>135062150</v>
@@ -3954,7 +3954,7 @@
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>221</v>
+        <v>62</v>
       </c>
       <c r="B64" t="n">
         <v>135292152</v>
@@ -3996,7 +3996,7 @@
         <v>-16</v>
       </c>
       <c r="O64" t="n">
-        <v>-7</v>
+        <v>78</v>
       </c>
       <c r="P64" t="n">
         <v>720000</v>
@@ -4010,7 +4010,7 @@
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>222</v>
+        <v>63</v>
       </c>
       <c r="B65" t="n">
         <v>135292168</v>
@@ -4066,7 +4066,7 @@
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>223</v>
+        <v>64</v>
       </c>
       <c r="B66" t="n">
         <v>135292178</v>
@@ -4112,7 +4112,7 @@
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>229</v>
+        <v>65</v>
       </c>
       <c r="B67" t="n">
         <v>135292430</v>
@@ -4168,7 +4168,7 @@
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>236</v>
+        <v>66</v>
       </c>
       <c r="B68" t="n">
         <v>135320109</v>
@@ -4214,7 +4214,7 @@
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>238</v>
+        <v>67</v>
       </c>
       <c r="B69" t="n">
         <v>135320132</v>
@@ -4260,7 +4260,7 @@
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>239</v>
+        <v>68</v>
       </c>
       <c r="B70" t="n">
         <v>135320423</v>
@@ -4306,7 +4306,7 @@
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
-        <v>242</v>
+        <v>69</v>
       </c>
       <c r="B71" t="n">
         <v>135320904</v>
@@ -4362,7 +4362,7 @@
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
-        <v>243</v>
+        <v>70</v>
       </c>
       <c r="B72" t="n">
         <v>135320905</v>
@@ -4408,7 +4408,7 @@
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
-        <v>244</v>
+        <v>71</v>
       </c>
       <c r="B73" t="n">
         <v>135320906</v>
@@ -4464,7 +4464,7 @@
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
-        <v>246</v>
+        <v>72</v>
       </c>
       <c r="B74" t="n">
         <v>135321602</v>
@@ -4514,7 +4514,7 @@
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
-        <v>247</v>
+        <v>73</v>
       </c>
       <c r="B75" t="n">
         <v>135321603</v>
@@ -4560,7 +4560,7 @@
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
-        <v>252</v>
+        <v>74</v>
       </c>
       <c r="B76" t="n">
         <v>135325102</v>
@@ -4616,7 +4616,7 @@
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
-        <v>256</v>
+        <v>75</v>
       </c>
       <c r="B77" t="n">
         <v>135900206</v>
@@ -4658,7 +4658,7 @@
         <v>-32</v>
       </c>
       <c r="O77" t="n">
-        <v>-28</v>
+        <v>62</v>
       </c>
       <c r="P77" t="n">
         <v>16000</v>
@@ -4672,7 +4672,7 @@
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
-        <v>266</v>
+        <v>76</v>
       </c>
       <c r="B78" t="n">
         <v>136130101</v>
@@ -4728,7 +4728,7 @@
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
-        <v>267</v>
+        <v>77</v>
       </c>
       <c r="B79" t="n">
         <v>136130102</v>
@@ -4784,7 +4784,7 @@
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
-        <v>270</v>
+        <v>78</v>
       </c>
       <c r="B80" t="n">
         <v>136170112</v>
@@ -4840,7 +4840,7 @@
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
-        <v>273</v>
+        <v>79</v>
       </c>
       <c r="B81" t="n">
         <v>136170115</v>
@@ -4896,7 +4896,7 @@
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
-        <v>276</v>
+        <v>80</v>
       </c>
       <c r="B82" t="n">
         <v>136170121</v>
@@ -4952,7 +4952,7 @@
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
-        <v>278</v>
+        <v>81</v>
       </c>
       <c r="B83" t="n">
         <v>136170151</v>
@@ -4994,7 +4994,7 @@
         <v>-58</v>
       </c>
       <c r="O83" t="n">
-        <v>-6</v>
+        <v>36</v>
       </c>
       <c r="P83" t="n">
         <v>99000</v>
@@ -5008,7 +5008,7 @@
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
-        <v>279</v>
+        <v>82</v>
       </c>
       <c r="B84" t="n">
         <v>136170152</v>
@@ -5064,7 +5064,7 @@
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
-        <v>280</v>
+        <v>83</v>
       </c>
       <c r="B85" t="n">
         <v>136170153</v>
@@ -5106,7 +5106,7 @@
         <v>-57</v>
       </c>
       <c r="O85" t="n">
-        <v>-3</v>
+        <v>37</v>
       </c>
       <c r="P85" t="n">
         <v>132000</v>
@@ -5120,7 +5120,7 @@
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
-        <v>281</v>
+        <v>84</v>
       </c>
       <c r="B86" t="n">
         <v>136170154</v>
@@ -5176,7 +5176,7 @@
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
-        <v>284</v>
+        <v>85</v>
       </c>
       <c r="B87" t="n">
         <v>136170157</v>
@@ -5232,7 +5232,7 @@
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
-        <v>286</v>
+        <v>86</v>
       </c>
       <c r="B88" t="n">
         <v>136170180</v>
@@ -5288,7 +5288,7 @@
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
-        <v>287</v>
+        <v>87</v>
       </c>
       <c r="B89" t="n">
         <v>136170182</v>
@@ -5338,7 +5338,7 @@
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
-        <v>288</v>
+        <v>88</v>
       </c>
       <c r="B90" t="n">
         <v>136170183</v>
@@ -5380,7 +5380,7 @@
         <v>-29</v>
       </c>
       <c r="O90" t="n">
-        <v>-23</v>
+        <v>65</v>
       </c>
       <c r="P90" t="n">
         <v>11000</v>
@@ -5394,7 +5394,7 @@
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
-        <v>289</v>
+        <v>89</v>
       </c>
       <c r="B91" t="n">
         <v>136170185</v>
@@ -5450,7 +5450,7 @@
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
-        <v>290</v>
+        <v>90</v>
       </c>
       <c r="B92" t="n">
         <v>136170186</v>
@@ -5506,7 +5506,7 @@
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
-        <v>295</v>
+        <v>91</v>
       </c>
       <c r="B93" t="n">
         <v>136170225</v>
@@ -5552,7 +5552,7 @@
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
-        <v>299</v>
+        <v>92</v>
       </c>
       <c r="B94" t="n">
         <v>136170243</v>
@@ -5598,7 +5598,7 @@
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
-        <v>302</v>
+        <v>93</v>
       </c>
       <c r="B95" t="n">
         <v>136170330</v>
@@ -5654,7 +5654,7 @@
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
-        <v>303</v>
+        <v>94</v>
       </c>
       <c r="B96" t="n">
         <v>136170331</v>
@@ -5696,7 +5696,7 @@
         <v>-40</v>
       </c>
       <c r="O96" t="n">
-        <v>-20</v>
+        <v>54</v>
       </c>
       <c r="P96" t="n">
         <v>88000</v>
@@ -5710,7 +5710,7 @@
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
-        <v>304</v>
+        <v>95</v>
       </c>
       <c r="B97" t="n">
         <v>136170332</v>
@@ -5766,7 +5766,7 @@
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
-        <v>306</v>
+        <v>96</v>
       </c>
       <c r="B98" t="n">
         <v>136170334</v>
@@ -5822,7 +5822,7 @@
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
-        <v>310</v>
+        <v>97</v>
       </c>
       <c r="B99" t="n">
         <v>136170345</v>
@@ -5868,7 +5868,7 @@
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
-        <v>312</v>
+        <v>98</v>
       </c>
       <c r="B100" t="n">
         <v>136175002</v>
@@ -5910,7 +5910,7 @@
         <v>172</v>
       </c>
       <c r="O100" t="n">
-        <v>-28</v>
+        <v>266</v>
       </c>
       <c r="P100" t="n">
         <v>16000</v>
@@ -5924,7 +5924,7 @@
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
-        <v>320</v>
+        <v>99</v>
       </c>
       <c r="B101" t="n">
         <v>136176037</v>
@@ -5970,7 +5970,7 @@
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
-        <v>321</v>
+        <v>100</v>
       </c>
       <c r="B102" t="n">
         <v>136176046</v>
@@ -6016,7 +6016,7 @@
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
-        <v>324</v>
+        <v>101</v>
       </c>
       <c r="B103" t="n">
         <v>136176097</v>
@@ -6062,7 +6062,7 @@
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
-        <v>326</v>
+        <v>102</v>
       </c>
       <c r="B104" t="n">
         <v>136178304</v>
@@ -6118,7 +6118,7 @@
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
-        <v>342</v>
+        <v>103</v>
       </c>
       <c r="B105" t="n">
         <v>136910303</v>
@@ -6174,7 +6174,7 @@
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
-        <v>343</v>
+        <v>104</v>
       </c>
       <c r="B106" t="n">
         <v>136910501</v>
@@ -6230,7 +6230,7 @@
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
-        <v>344</v>
+        <v>105</v>
       </c>
       <c r="B107" t="n">
         <v>136910505</v>
@@ -6276,7 +6276,7 @@
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
-        <v>345</v>
+        <v>106</v>
       </c>
       <c r="B108" t="n">
         <v>136910701</v>
@@ -6318,7 +6318,7 @@
         <v>-44</v>
       </c>
       <c r="O108" t="n">
-        <v>-2</v>
+        <v>50</v>
       </c>
       <c r="P108" t="n">
         <v>81000</v>
@@ -6332,7 +6332,7 @@
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
-        <v>346</v>
+        <v>107</v>
       </c>
       <c r="B109" t="n">
         <v>136910703</v>
@@ -6378,7 +6378,7 @@
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
-        <v>347</v>
+        <v>108</v>
       </c>
       <c r="B110" t="n">
         <v>136911001</v>
@@ -6434,7 +6434,7 @@
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
-        <v>348</v>
+        <v>109</v>
       </c>
       <c r="B111" t="n">
         <v>136911003</v>
@@ -6480,7 +6480,7 @@
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
-        <v>358</v>
+        <v>110</v>
       </c>
       <c r="B112" t="n">
         <v>143100152</v>
@@ -6536,7 +6536,7 @@
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
-        <v>360</v>
+        <v>111</v>
       </c>
       <c r="B113" t="n">
         <v>143100154</v>
@@ -6592,7 +6592,7 @@
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
-        <v>362</v>
+        <v>112</v>
       </c>
       <c r="B114" t="n">
         <v>143100156</v>
@@ -6648,7 +6648,7 @@
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
-        <v>363</v>
+        <v>113</v>
       </c>
       <c r="B115" t="n">
         <v>143100157</v>
@@ -6704,7 +6704,7 @@
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
-        <v>365</v>
+        <v>114</v>
       </c>
       <c r="B116" t="n">
         <v>143100159</v>
@@ -6760,7 +6760,7 @@
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
-        <v>374</v>
+        <v>115</v>
       </c>
       <c r="B117" t="n">
         <v>143120221</v>
@@ -6816,7 +6816,7 @@
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
-        <v>375</v>
+        <v>116</v>
       </c>
       <c r="B118" t="n">
         <v>143120222</v>
@@ -6862,7 +6862,7 @@
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
-        <v>376</v>
+        <v>117</v>
       </c>
       <c r="B119" t="n">
         <v>143120223</v>
@@ -6908,7 +6908,7 @@
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
-        <v>377</v>
+        <v>118</v>
       </c>
       <c r="B120" t="n">
         <v>143120225</v>
@@ -6964,7 +6964,7 @@
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
-        <v>383</v>
+        <v>119</v>
       </c>
       <c r="B121" t="n">
         <v>143130109</v>
@@ -7006,7 +7006,7 @@
         <v>-52</v>
       </c>
       <c r="O121" t="n">
-        <v>-12</v>
+        <v>42</v>
       </c>
       <c r="P121" t="n">
         <v>5472000</v>
@@ -7020,7 +7020,7 @@
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
-        <v>384</v>
+        <v>120</v>
       </c>
       <c r="B122" t="n">
         <v>143130110</v>
@@ -7052,7 +7052,7 @@
         <v>397</v>
       </c>
       <c r="O122" t="n">
-        <v>-20</v>
+        <v>491</v>
       </c>
       <c r="P122" t="n">
         <v>288000</v>
@@ -7066,7 +7066,7 @@
     </row>
     <row r="123">
       <c r="A123" s="1" t="n">
-        <v>389</v>
+        <v>121</v>
       </c>
       <c r="B123" t="n">
         <v>143131023</v>
@@ -7108,7 +7108,7 @@
         <v>-61</v>
       </c>
       <c r="O123" t="n">
-        <v>-2</v>
+        <v>33</v>
       </c>
       <c r="P123" t="n">
         <v>10560000</v>
@@ -7122,7 +7122,7 @@
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
-        <v>391</v>
+        <v>122</v>
       </c>
       <c r="B124" t="n">
         <v>143131025</v>
@@ -7178,7 +7178,7 @@
     </row>
     <row r="125">
       <c r="A125" s="1" t="n">
-        <v>392</v>
+        <v>123</v>
       </c>
       <c r="B125" t="n">
         <v>143133113</v>
@@ -7224,7 +7224,7 @@
     </row>
     <row r="126">
       <c r="A126" s="1" t="n">
-        <v>396</v>
+        <v>124</v>
       </c>
       <c r="B126" t="n">
         <v>143170134</v>
@@ -7280,7 +7280,7 @@
     </row>
     <row r="127">
       <c r="A127" s="1" t="n">
-        <v>408</v>
+        <v>125</v>
       </c>
       <c r="B127" t="n">
         <v>152023010</v>
@@ -7310,7 +7310,7 @@
         <v>807</v>
       </c>
       <c r="O127" t="n">
-        <v>-462</v>
+        <v>901</v>
       </c>
       <c r="P127" t="n">
         <v>64000</v>
@@ -7324,7 +7324,7 @@
     </row>
     <row r="128">
       <c r="A128" s="1" t="n">
-        <v>413</v>
+        <v>126</v>
       </c>
       <c r="B128" t="n">
         <v>152023017</v>
@@ -7380,7 +7380,7 @@
     </row>
     <row r="129">
       <c r="A129" s="1" t="n">
-        <v>418</v>
+        <v>127</v>
       </c>
       <c r="B129" t="n">
         <v>152023024</v>
@@ -7412,7 +7412,7 @@
         <v>-8</v>
       </c>
       <c r="O129" t="n">
-        <v>-38</v>
+        <v>86</v>
       </c>
       <c r="P129" t="n">
         <v>240000</v>
@@ -7426,7 +7426,7 @@
     </row>
     <row r="130">
       <c r="A130" s="1" t="n">
-        <v>419</v>
+        <v>128</v>
       </c>
       <c r="B130" t="n">
         <v>152023025</v>
@@ -7472,7 +7472,7 @@
     </row>
     <row r="131">
       <c r="A131" s="1" t="n">
-        <v>421</v>
+        <v>129</v>
       </c>
       <c r="B131" t="n">
         <v>152023027</v>
@@ -7518,7 +7518,7 @@
     </row>
     <row r="132">
       <c r="A132" s="1" t="n">
-        <v>422</v>
+        <v>130</v>
       </c>
       <c r="B132" t="n">
         <v>152023028</v>
@@ -7550,7 +7550,7 @@
         <v>-57</v>
       </c>
       <c r="O132" t="n">
-        <v>-3</v>
+        <v>37</v>
       </c>
       <c r="P132" t="n">
         <v>1040000</v>
@@ -7564,7 +7564,7 @@
     </row>
     <row r="133">
       <c r="A133" s="1" t="n">
-        <v>423</v>
+        <v>131</v>
       </c>
       <c r="B133" t="n">
         <v>152023029</v>
@@ -7596,7 +7596,7 @@
         <v>-46</v>
       </c>
       <c r="O133" t="n">
-        <v>-6</v>
+        <v>48</v>
       </c>
       <c r="P133" t="n">
         <v>80000</v>
@@ -7610,7 +7610,7 @@
     </row>
     <row r="134">
       <c r="A134" s="1" t="n">
-        <v>424</v>
+        <v>132</v>
       </c>
       <c r="B134" t="n">
         <v>152023030</v>
@@ -7656,7 +7656,7 @@
     </row>
     <row r="135">
       <c r="A135" s="1" t="n">
-        <v>425</v>
+        <v>133</v>
       </c>
       <c r="B135" t="n">
         <v>152023031</v>
@@ -7702,7 +7702,7 @@
     </row>
     <row r="136">
       <c r="A136" s="1" t="n">
-        <v>434</v>
+        <v>134</v>
       </c>
       <c r="B136" t="n">
         <v>152270226</v>
@@ -7744,7 +7744,7 @@
         <v>-59</v>
       </c>
       <c r="O136" t="n">
-        <v>-1</v>
+        <v>35</v>
       </c>
       <c r="P136" t="n">
         <v>320000</v>
@@ -7758,7 +7758,7 @@
     </row>
     <row r="137">
       <c r="A137" s="1" t="n">
-        <v>435</v>
+        <v>135</v>
       </c>
       <c r="B137" t="n">
         <v>152270228</v>
@@ -7814,7 +7814,7 @@
     </row>
     <row r="138">
       <c r="A138" s="1" t="n">
-        <v>436</v>
+        <v>136</v>
       </c>
       <c r="B138" t="n">
         <v>152270229</v>
@@ -7870,7 +7870,7 @@
     </row>
     <row r="139">
       <c r="A139" s="1" t="n">
-        <v>437</v>
+        <v>137</v>
       </c>
       <c r="B139" t="n">
         <v>152270232</v>
@@ -7926,7 +7926,7 @@
     </row>
     <row r="140">
       <c r="A140" s="1" t="n">
-        <v>439</v>
+        <v>138</v>
       </c>
       <c r="B140" t="n">
         <v>152270234</v>
@@ -7982,7 +7982,7 @@
     </row>
     <row r="141">
       <c r="A141" s="1" t="n">
-        <v>442</v>
+        <v>139</v>
       </c>
       <c r="B141" t="n">
         <v>152270322</v>
@@ -8038,7 +8038,7 @@
     </row>
     <row r="142">
       <c r="A142" s="1" t="n">
-        <v>444</v>
+        <v>140</v>
       </c>
       <c r="B142" t="n">
         <v>152270336</v>
@@ -8094,7 +8094,7 @@
     </row>
     <row r="143">
       <c r="A143" s="1" t="n">
-        <v>445</v>
+        <v>141</v>
       </c>
       <c r="B143" t="n">
         <v>152270337</v>
@@ -8150,7 +8150,7 @@
     </row>
     <row r="144">
       <c r="A144" s="1" t="n">
-        <v>447</v>
+        <v>142</v>
       </c>
       <c r="B144" t="n">
         <v>152270339</v>
@@ -8206,7 +8206,7 @@
     </row>
     <row r="145">
       <c r="A145" s="1" t="n">
-        <v>448</v>
+        <v>143</v>
       </c>
       <c r="B145" t="n">
         <v>152270340</v>
@@ -8262,7 +8262,7 @@
     </row>
     <row r="146">
       <c r="A146" s="1" t="n">
-        <v>451</v>
+        <v>144</v>
       </c>
       <c r="B146" t="n">
         <v>152270344</v>
@@ -8318,7 +8318,7 @@
     </row>
     <row r="147">
       <c r="A147" s="1" t="n">
-        <v>452</v>
+        <v>145</v>
       </c>
       <c r="B147" t="n">
         <v>152270346</v>
@@ -8374,7 +8374,7 @@
     </row>
     <row r="148">
       <c r="A148" s="1" t="n">
-        <v>453</v>
+        <v>146</v>
       </c>
       <c r="B148" t="n">
         <v>152270347</v>
@@ -8406,7 +8406,7 @@
         <v>-58</v>
       </c>
       <c r="O148" t="n">
-        <v>-3</v>
+        <v>36</v>
       </c>
       <c r="P148" t="n">
         <v>400000</v>
@@ -8420,7 +8420,7 @@
     </row>
     <row r="149">
       <c r="A149" s="1" t="n">
-        <v>454</v>
+        <v>147</v>
       </c>
       <c r="B149" t="n">
         <v>152290201</v>
@@ -8476,7 +8476,7 @@
     </row>
     <row r="150">
       <c r="A150" s="1" t="n">
-        <v>455</v>
+        <v>148</v>
       </c>
       <c r="B150" t="n">
         <v>152290202</v>
@@ -8532,7 +8532,7 @@
     </row>
     <row r="151">
       <c r="A151" s="1" t="n">
-        <v>456</v>
+        <v>149</v>
       </c>
       <c r="B151" t="n">
         <v>152290203</v>
@@ -8574,7 +8574,7 @@
         <v>-61</v>
       </c>
       <c r="O151" t="n">
-        <v>-3</v>
+        <v>33</v>
       </c>
       <c r="P151" t="n">
         <v>2400000</v>
@@ -8588,7 +8588,7 @@
     </row>
     <row r="152">
       <c r="A152" s="1" t="n">
-        <v>458</v>
+        <v>150</v>
       </c>
       <c r="B152" t="n">
         <v>152290208</v>
@@ -8644,7 +8644,7 @@
     </row>
     <row r="153">
       <c r="A153" s="1" t="n">
-        <v>459</v>
+        <v>151</v>
       </c>
       <c r="B153" t="n">
         <v>152290209</v>
@@ -8700,7 +8700,7 @@
     </row>
     <row r="154">
       <c r="A154" s="1" t="n">
-        <v>461</v>
+        <v>152</v>
       </c>
       <c r="B154" t="n">
         <v>152290216</v>
@@ -8756,7 +8756,7 @@
     </row>
     <row r="155">
       <c r="A155" s="1" t="n">
-        <v>463</v>
+        <v>153</v>
       </c>
       <c r="B155" t="n">
         <v>152290218</v>
@@ -8802,7 +8802,7 @@
     </row>
     <row r="156">
       <c r="A156" s="1" t="n">
-        <v>464</v>
+        <v>154</v>
       </c>
       <c r="B156" t="n">
         <v>152320101</v>
@@ -8858,7 +8858,7 @@
     </row>
     <row r="157">
       <c r="A157" s="1" t="n">
-        <v>468</v>
+        <v>155</v>
       </c>
       <c r="B157" t="n">
         <v>152320107</v>
@@ -8892,7 +8892,7 @@
     </row>
     <row r="158">
       <c r="A158" s="1" t="n">
-        <v>470</v>
+        <v>156</v>
       </c>
       <c r="B158" t="n">
         <v>152320112</v>
@@ -8948,7 +8948,7 @@
     </row>
     <row r="159">
       <c r="A159" s="1" t="n">
-        <v>472</v>
+        <v>157</v>
       </c>
       <c r="B159" t="n">
         <v>152320115</v>
@@ -9004,7 +9004,7 @@
     </row>
     <row r="160">
       <c r="A160" s="1" t="n">
-        <v>473</v>
+        <v>158</v>
       </c>
       <c r="B160" t="n">
         <v>152320119</v>
@@ -9046,7 +9046,7 @@
         <v>-54</v>
       </c>
       <c r="O160" t="n">
-        <v>-10</v>
+        <v>40</v>
       </c>
       <c r="P160" t="n">
         <v>880000</v>
@@ -9060,7 +9060,7 @@
     </row>
     <row r="161">
       <c r="A161" s="1" t="n">
-        <v>475</v>
+        <v>159</v>
       </c>
       <c r="B161" t="n">
         <v>152320124</v>
@@ -9116,7 +9116,7 @@
     </row>
     <row r="162">
       <c r="A162" s="1" t="n">
-        <v>476</v>
+        <v>160</v>
       </c>
       <c r="B162" t="n">
         <v>152320137</v>
@@ -9172,7 +9172,7 @@
     </row>
     <row r="163">
       <c r="A163" s="1" t="n">
-        <v>479</v>
+        <v>161</v>
       </c>
       <c r="B163" t="n">
         <v>152320155</v>
@@ -9228,7 +9228,7 @@
     </row>
     <row r="164">
       <c r="A164" s="1" t="n">
-        <v>480</v>
+        <v>162</v>
       </c>
       <c r="B164" t="n">
         <v>152320156</v>
@@ -9284,7 +9284,7 @@
     </row>
     <row r="165">
       <c r="A165" s="1" t="n">
-        <v>484</v>
+        <v>163</v>
       </c>
       <c r="B165" t="n">
         <v>152320164</v>
@@ -9340,7 +9340,7 @@
     </row>
     <row r="166">
       <c r="A166" s="1" t="n">
-        <v>485</v>
+        <v>164</v>
       </c>
       <c r="B166" t="n">
         <v>152320165</v>
@@ -9382,7 +9382,7 @@
         <v>-16</v>
       </c>
       <c r="O166" t="n">
-        <v>-44</v>
+        <v>78</v>
       </c>
       <c r="P166" t="n">
         <v>240000</v>
@@ -9396,7 +9396,7 @@
     </row>
     <row r="167">
       <c r="A167" s="1" t="n">
-        <v>487</v>
+        <v>165</v>
       </c>
       <c r="B167" t="n">
         <v>152320173</v>
@@ -9452,7 +9452,7 @@
     </row>
     <row r="168">
       <c r="A168" s="1" t="n">
-        <v>489</v>
+        <v>166</v>
       </c>
       <c r="B168" t="n">
         <v>152320181</v>
@@ -9508,7 +9508,7 @@
     </row>
     <row r="169">
       <c r="A169" s="1" t="n">
-        <v>495</v>
+        <v>167</v>
       </c>
       <c r="B169" t="n">
         <v>152320188</v>
@@ -9564,7 +9564,7 @@
     </row>
     <row r="170">
       <c r="A170" s="1" t="n">
-        <v>497</v>
+        <v>168</v>
       </c>
       <c r="B170" t="n">
         <v>152350101</v>
@@ -9606,7 +9606,7 @@
         <v>-58</v>
       </c>
       <c r="O170" t="n">
-        <v>-6</v>
+        <v>36</v>
       </c>
       <c r="P170" t="n">
         <v>2867200</v>
@@ -9620,7 +9620,7 @@
     </row>
     <row r="171">
       <c r="A171" s="1" t="n">
-        <v>499</v>
+        <v>169</v>
       </c>
       <c r="B171" t="n">
         <v>152350105</v>
@@ -9676,7 +9676,7 @@
     </row>
     <row r="172">
       <c r="A172" s="1" t="n">
-        <v>501</v>
+        <v>170</v>
       </c>
       <c r="B172" t="n">
         <v>152350110</v>
@@ -9722,7 +9722,7 @@
     </row>
     <row r="173">
       <c r="A173" s="1" t="n">
-        <v>508</v>
+        <v>171</v>
       </c>
       <c r="B173" t="n">
         <v>152420158</v>
@@ -9778,7 +9778,7 @@
     </row>
     <row r="174">
       <c r="A174" s="1" t="n">
-        <v>511</v>
+        <v>172</v>
       </c>
       <c r="B174" t="n">
         <v>152420161</v>
@@ -9820,7 +9820,7 @@
         <v>-60</v>
       </c>
       <c r="O174" t="n">
-        <v>-1</v>
+        <v>34</v>
       </c>
       <c r="P174" t="n">
         <v>1480000</v>
@@ -9834,7 +9834,7 @@
     </row>
     <row r="175">
       <c r="A175" s="1" t="n">
-        <v>512</v>
+        <v>173</v>
       </c>
       <c r="B175" t="n">
         <v>152420163</v>
@@ -9890,7 +9890,7 @@
     </row>
     <row r="176">
       <c r="A176" s="1" t="n">
-        <v>513</v>
+        <v>174</v>
       </c>
       <c r="B176" t="n">
         <v>152420164</v>
@@ -9946,7 +9946,7 @@
     </row>
     <row r="177">
       <c r="A177" s="1" t="n">
-        <v>514</v>
+        <v>175</v>
       </c>
       <c r="B177" t="n">
         <v>152420165</v>
@@ -10002,7 +10002,7 @@
     </row>
     <row r="178">
       <c r="A178" s="1" t="n">
-        <v>515</v>
+        <v>176</v>
       </c>
       <c r="B178" t="n">
         <v>152420166</v>
@@ -10058,7 +10058,7 @@
     </row>
     <row r="179">
       <c r="A179" s="1" t="n">
-        <v>516</v>
+        <v>177</v>
       </c>
       <c r="B179" t="n">
         <v>152420167</v>
@@ -10104,7 +10104,7 @@
     </row>
     <row r="180">
       <c r="A180" s="1" t="n">
-        <v>518</v>
+        <v>178</v>
       </c>
       <c r="B180" t="n">
         <v>152421052</v>
@@ -10160,7 +10160,7 @@
     </row>
     <row r="181">
       <c r="A181" s="1" t="n">
-        <v>519</v>
+        <v>179</v>
       </c>
       <c r="B181" t="n">
         <v>152421053</v>
@@ -10202,7 +10202,7 @@
         <v>122</v>
       </c>
       <c r="O181" t="n">
-        <v>-158</v>
+        <v>216</v>
       </c>
       <c r="P181" t="n">
         <v>256000</v>
@@ -10216,7 +10216,7 @@
     </row>
     <row r="182">
       <c r="A182" s="1" t="n">
-        <v>522</v>
+        <v>180</v>
       </c>
       <c r="B182" t="n">
         <v>152430152</v>
@@ -10272,7 +10272,7 @@
     </row>
     <row r="183">
       <c r="A183" s="1" t="n">
-        <v>525</v>
+        <v>181</v>
       </c>
       <c r="B183" t="n">
         <v>152430155</v>
@@ -10304,7 +10304,7 @@
         <v>-29</v>
       </c>
       <c r="O183" t="n">
-        <v>-35</v>
+        <v>65</v>
       </c>
       <c r="P183" t="n">
         <v>2550000</v>
@@ -10318,7 +10318,7 @@
     </row>
     <row r="184">
       <c r="A184" s="1" t="n">
-        <v>526</v>
+        <v>182</v>
       </c>
       <c r="B184" t="n">
         <v>152430158</v>
@@ -10360,7 +10360,7 @@
         <v>-47</v>
       </c>
       <c r="O184" t="n">
-        <v>-14</v>
+        <v>47</v>
       </c>
       <c r="P184" t="n">
         <v>1600000</v>
@@ -10374,7 +10374,7 @@
     </row>
     <row r="185">
       <c r="A185" s="1" t="n">
-        <v>527</v>
+        <v>183</v>
       </c>
       <c r="B185" t="n">
         <v>152430159</v>
@@ -10430,7 +10430,7 @@
     </row>
     <row r="186">
       <c r="A186" s="1" t="n">
-        <v>528</v>
+        <v>184</v>
       </c>
       <c r="B186" t="n">
         <v>152430160</v>
@@ -10486,7 +10486,7 @@
     </row>
     <row r="187">
       <c r="A187" s="1" t="n">
-        <v>531</v>
+        <v>185</v>
       </c>
       <c r="B187" t="n">
         <v>152440128</v>
@@ -10532,7 +10532,7 @@
     </row>
     <row r="188">
       <c r="A188" s="1" t="n">
-        <v>533</v>
+        <v>186</v>
       </c>
       <c r="B188" t="n">
         <v>152440130</v>
@@ -10578,7 +10578,7 @@
     </row>
     <row r="189">
       <c r="A189" s="1" t="n">
-        <v>546</v>
+        <v>187</v>
       </c>
       <c r="B189" t="n">
         <v>152440201</v>
@@ -10620,7 +10620,7 @@
         <v>-52</v>
       </c>
       <c r="O189" t="n">
-        <v>-5</v>
+        <v>42</v>
       </c>
       <c r="P189" t="n">
         <v>3162000</v>
@@ -10634,7 +10634,7 @@
     </row>
     <row r="190">
       <c r="A190" s="1" t="n">
-        <v>547</v>
+        <v>188</v>
       </c>
       <c r="B190" t="n">
         <v>152440202</v>
@@ -10676,7 +10676,7 @@
         <v>-61</v>
       </c>
       <c r="O190" t="n">
-        <v>-3</v>
+        <v>33</v>
       </c>
       <c r="P190" t="n">
         <v>494700</v>
@@ -10690,7 +10690,7 @@
     </row>
     <row r="191">
       <c r="A191" s="1" t="n">
-        <v>550</v>
+        <v>189</v>
       </c>
       <c r="B191" t="n">
         <v>152440205</v>
@@ -10746,7 +10746,7 @@
     </row>
     <row r="192">
       <c r="A192" s="1" t="n">
-        <v>551</v>
+        <v>190</v>
       </c>
       <c r="B192" t="n">
         <v>152440206</v>
@@ -10802,7 +10802,7 @@
     </row>
     <row r="193">
       <c r="A193" s="1" t="n">
-        <v>552</v>
+        <v>191</v>
       </c>
       <c r="B193" t="n">
         <v>152440207</v>
@@ -10858,7 +10858,7 @@
     </row>
     <row r="194">
       <c r="A194" s="1" t="n">
-        <v>553</v>
+        <v>192</v>
       </c>
       <c r="B194" t="n">
         <v>152440208</v>
@@ -10914,7 +10914,7 @@
     </row>
     <row r="195">
       <c r="A195" s="1" t="n">
-        <v>560</v>
+        <v>193</v>
       </c>
       <c r="B195" t="n">
         <v>152510101</v>
@@ -10970,7 +10970,7 @@
     </row>
     <row r="196">
       <c r="A196" s="1" t="n">
-        <v>563</v>
+        <v>194</v>
       </c>
       <c r="B196" t="n">
         <v>152510106</v>
@@ -11026,7 +11026,7 @@
     </row>
     <row r="197">
       <c r="A197" s="1" t="n">
-        <v>564</v>
+        <v>195</v>
       </c>
       <c r="B197" t="n">
         <v>152510107</v>
@@ -11082,7 +11082,7 @@
     </row>
     <row r="198">
       <c r="A198" s="1" t="n">
-        <v>568</v>
+        <v>196</v>
       </c>
       <c r="B198" t="n">
         <v>153010112</v>
@@ -11138,7 +11138,7 @@
     </row>
     <row r="199">
       <c r="A199" s="1" t="n">
-        <v>569</v>
+        <v>197</v>
       </c>
       <c r="B199" t="n">
         <v>153010114</v>
@@ -11180,7 +11180,7 @@
         <v>-47</v>
       </c>
       <c r="O199" t="n">
-        <v>-6</v>
+        <v>47</v>
       </c>
       <c r="P199" t="n">
         <v>88000</v>
@@ -11194,7 +11194,7 @@
     </row>
     <row r="200">
       <c r="A200" s="1" t="n">
-        <v>570</v>
+        <v>198</v>
       </c>
       <c r="B200" t="n">
         <v>153010115</v>
@@ -11250,7 +11250,7 @@
     </row>
     <row r="201">
       <c r="A201" s="1" t="n">
-        <v>573</v>
+        <v>199</v>
       </c>
       <c r="B201" t="n">
         <v>153010225</v>
@@ -11306,7 +11306,7 @@
     </row>
     <row r="202">
       <c r="A202" s="1" t="n">
-        <v>580</v>
+        <v>200</v>
       </c>
       <c r="B202" t="n">
         <v>153010311</v>
@@ -11362,7 +11362,7 @@
     </row>
     <row r="203">
       <c r="A203" s="1" t="n">
-        <v>582</v>
+        <v>201</v>
       </c>
       <c r="B203" t="n">
         <v>153100208</v>
@@ -11418,7 +11418,7 @@
     </row>
     <row r="204">
       <c r="A204" s="1" t="n">
-        <v>583</v>
+        <v>202</v>
       </c>
       <c r="B204" t="n">
         <v>153100213</v>
@@ -11460,7 +11460,7 @@
         <v>-4</v>
       </c>
       <c r="O204" t="n">
-        <v>-57</v>
+        <v>90</v>
       </c>
       <c r="P204" t="n">
         <v>50000</v>
@@ -11474,7 +11474,7 @@
     </row>
     <row r="205">
       <c r="A205" s="1" t="n">
-        <v>589</v>
+        <v>203</v>
       </c>
       <c r="B205" t="n">
         <v>153100452</v>
@@ -11530,7 +11530,7 @@
     </row>
     <row r="206">
       <c r="A206" s="1" t="n">
-        <v>590</v>
+        <v>204</v>
       </c>
       <c r="B206" t="n">
         <v>153100453</v>
@@ -11586,7 +11586,7 @@
     </row>
     <row r="207">
       <c r="A207" s="1" t="n">
-        <v>591</v>
+        <v>205</v>
       </c>
       <c r="B207" t="n">
         <v>153100454</v>
@@ -11642,7 +11642,7 @@
     </row>
     <row r="208">
       <c r="A208" s="1" t="n">
-        <v>592</v>
+        <v>206</v>
       </c>
       <c r="B208" t="n">
         <v>153100458</v>
@@ -11698,7 +11698,7 @@
     </row>
     <row r="209">
       <c r="A209" s="1" t="n">
-        <v>602</v>
+        <v>207</v>
       </c>
       <c r="B209" t="n">
         <v>153110143</v>
@@ -11754,7 +11754,7 @@
     </row>
     <row r="210">
       <c r="A210" s="1" t="n">
-        <v>603</v>
+        <v>208</v>
       </c>
       <c r="B210" t="n">
         <v>153110144</v>
@@ -11796,7 +11796,7 @@
         <v>-54</v>
       </c>
       <c r="O210" t="n">
-        <v>-6</v>
+        <v>40</v>
       </c>
       <c r="P210" t="n">
         <v>104000</v>
@@ -11810,7 +11810,7 @@
     </row>
     <row r="211">
       <c r="A211" s="1" t="n">
-        <v>607</v>
+        <v>209</v>
       </c>
       <c r="B211" t="n">
         <v>153110150</v>
@@ -11852,7 +11852,7 @@
         <v>-61</v>
       </c>
       <c r="O211" t="n">
-        <v>-3</v>
+        <v>33</v>
       </c>
       <c r="P211" t="n">
         <v>2904200</v>
@@ -11866,7 +11866,7 @@
     </row>
     <row r="212">
       <c r="A212" s="1" t="n">
-        <v>608</v>
+        <v>210</v>
       </c>
       <c r="B212" t="n">
         <v>153110151</v>
@@ -11908,7 +11908,7 @@
         <v>-33</v>
       </c>
       <c r="O212" t="n">
-        <v>-26</v>
+        <v>61</v>
       </c>
       <c r="P212" t="n">
         <v>104000</v>
@@ -11922,7 +11922,7 @@
     </row>
     <row r="213">
       <c r="A213" s="1" t="n">
-        <v>609</v>
+        <v>211</v>
       </c>
       <c r="B213" t="n">
         <v>153110152</v>
@@ -11978,7 +11978,7 @@
     </row>
     <row r="214">
       <c r="A214" s="1" t="n">
-        <v>612</v>
+        <v>212</v>
       </c>
       <c r="B214" t="n">
         <v>153110155</v>
@@ -12034,7 +12034,7 @@
     </row>
     <row r="215">
       <c r="A215" s="1" t="n">
-        <v>614</v>
+        <v>213</v>
       </c>
       <c r="B215" t="n">
         <v>153110157</v>
@@ -12090,7 +12090,7 @@
     </row>
     <row r="216">
       <c r="A216" s="1" t="n">
-        <v>616</v>
+        <v>214</v>
       </c>
       <c r="B216" t="n">
         <v>153110159</v>
@@ -12146,7 +12146,7 @@
     </row>
     <row r="217">
       <c r="A217" s="1" t="n">
-        <v>622</v>
+        <v>215</v>
       </c>
       <c r="B217" t="n">
         <v>154030107</v>
@@ -12202,7 +12202,7 @@
     </row>
     <row r="218">
       <c r="A218" s="1" t="n">
-        <v>629</v>
+        <v>216</v>
       </c>
       <c r="B218" t="n">
         <v>154030501</v>
@@ -12248,7 +12248,7 @@
     </row>
     <row r="219">
       <c r="A219" s="1" t="n">
-        <v>630</v>
+        <v>217</v>
       </c>
       <c r="B219" t="n">
         <v>154030502</v>
@@ -12280,7 +12280,7 @@
         <v>-54</v>
       </c>
       <c r="O219" t="n">
-        <v>-10</v>
+        <v>40</v>
       </c>
       <c r="P219" t="n">
         <v>603900</v>
@@ -12294,7 +12294,7 @@
     </row>
     <row r="220">
       <c r="A220" s="1" t="n">
-        <v>631</v>
+        <v>218</v>
       </c>
       <c r="B220" t="n">
         <v>154030503</v>
@@ -12340,7 +12340,7 @@
     </row>
     <row r="221">
       <c r="A221" s="1" t="n">
-        <v>632</v>
+        <v>219</v>
       </c>
       <c r="B221" t="n">
         <v>154030504</v>
@@ -12386,7 +12386,7 @@
     </row>
     <row r="222">
       <c r="A222" s="1" t="n">
-        <v>634</v>
+        <v>220</v>
       </c>
       <c r="B222" t="n">
         <v>154030506</v>
@@ -12432,7 +12432,7 @@
     </row>
     <row r="223">
       <c r="A223" s="1" t="n">
-        <v>635</v>
+        <v>221</v>
       </c>
       <c r="B223" t="n">
         <v>154040130</v>
@@ -12474,7 +12474,7 @@
         <v>-24</v>
       </c>
       <c r="O223" t="n">
-        <v>-2</v>
+        <v>70</v>
       </c>
       <c r="P223" t="n">
         <v>81600</v>
@@ -12488,7 +12488,7 @@
     </row>
     <row r="224">
       <c r="A224" s="1" t="n">
-        <v>636</v>
+        <v>222</v>
       </c>
       <c r="B224" t="n">
         <v>154040131</v>
@@ -12544,7 +12544,7 @@
     </row>
     <row r="225">
       <c r="A225" s="1" t="n">
-        <v>637</v>
+        <v>223</v>
       </c>
       <c r="B225" t="n">
         <v>154040201</v>
@@ -12600,7 +12600,7 @@
     </row>
     <row r="226">
       <c r="A226" s="1" t="n">
-        <v>638</v>
+        <v>224</v>
       </c>
       <c r="B226" t="n">
         <v>154040202</v>
@@ -12656,7 +12656,7 @@
     </row>
     <row r="227">
       <c r="A227" s="1" t="n">
-        <v>639</v>
+        <v>225</v>
       </c>
       <c r="B227" t="n">
         <v>154040203</v>
@@ -12712,7 +12712,7 @@
     </row>
     <row r="228">
       <c r="A228" s="1" t="n">
-        <v>640</v>
+        <v>226</v>
       </c>
       <c r="B228" t="n">
         <v>154040204</v>
@@ -12768,7 +12768,7 @@
     </row>
     <row r="229">
       <c r="A229" s="1" t="n">
-        <v>641</v>
+        <v>227</v>
       </c>
       <c r="B229" t="n">
         <v>154040205</v>
@@ -12810,7 +12810,7 @@
         <v>-59</v>
       </c>
       <c r="O229" t="n">
-        <v>-5</v>
+        <v>35</v>
       </c>
       <c r="P229" t="n">
         <v>438600</v>
@@ -12824,7 +12824,7 @@
     </row>
     <row r="230">
       <c r="A230" s="1" t="n">
-        <v>644</v>
+        <v>228</v>
       </c>
       <c r="B230" t="n">
         <v>154040217</v>
@@ -12866,7 +12866,7 @@
         <v>-61</v>
       </c>
       <c r="O230" t="n">
-        <v>-3</v>
+        <v>33</v>
       </c>
       <c r="P230" t="n">
         <v>1598000</v>
@@ -12880,7 +12880,7 @@
     </row>
     <row r="231">
       <c r="A231" s="1" t="n">
-        <v>645</v>
+        <v>229</v>
       </c>
       <c r="B231" t="n">
         <v>154040218</v>
@@ -12922,7 +12922,7 @@
         <v>-40</v>
       </c>
       <c r="O231" t="n">
-        <v>-5</v>
+        <v>54</v>
       </c>
       <c r="P231" t="n">
         <v>850000</v>
@@ -12936,7 +12936,7 @@
     </row>
     <row r="232">
       <c r="A232" s="1" t="n">
-        <v>646</v>
+        <v>230</v>
       </c>
       <c r="B232" t="n">
         <v>154040219</v>
@@ -12992,7 +12992,7 @@
     </row>
     <row r="233">
       <c r="A233" s="1" t="n">
-        <v>647</v>
+        <v>231</v>
       </c>
       <c r="B233" t="n">
         <v>154040220</v>
@@ -13048,7 +13048,7 @@
     </row>
     <row r="234">
       <c r="A234" s="1" t="n">
-        <v>649</v>
+        <v>232</v>
       </c>
       <c r="B234" t="n">
         <v>154040225</v>
@@ -13104,7 +13104,7 @@
     </row>
     <row r="235">
       <c r="A235" s="1" t="n">
-        <v>653</v>
+        <v>233</v>
       </c>
       <c r="B235" t="n">
         <v>154040234</v>
@@ -13160,7 +13160,7 @@
     </row>
     <row r="236">
       <c r="A236" s="1" t="n">
-        <v>655</v>
+        <v>234</v>
       </c>
       <c r="B236" t="n">
         <v>154040237</v>
@@ -13216,7 +13216,7 @@
     </row>
     <row r="237">
       <c r="A237" s="1" t="n">
-        <v>656</v>
+        <v>235</v>
       </c>
       <c r="B237" t="n">
         <v>154040238</v>
@@ -13272,7 +13272,7 @@
     </row>
     <row r="238">
       <c r="A238" s="1" t="n">
-        <v>658</v>
+        <v>236</v>
       </c>
       <c r="B238" t="n">
         <v>154040240</v>
@@ -13318,7 +13318,7 @@
     </row>
     <row r="239">
       <c r="A239" s="1" t="n">
-        <v>663</v>
+        <v>237</v>
       </c>
       <c r="B239" t="n">
         <v>154040245</v>
@@ -13360,7 +13360,7 @@
         <v>-47</v>
       </c>
       <c r="O239" t="n">
-        <v>-6</v>
+        <v>47</v>
       </c>
       <c r="P239" t="n">
         <v>408000</v>
@@ -13374,7 +13374,7 @@
     </row>
     <row r="240">
       <c r="A240" s="1" t="n">
-        <v>668</v>
+        <v>238</v>
       </c>
       <c r="B240" t="n">
         <v>170491227</v>
@@ -13420,7 +13420,7 @@
     </row>
     <row r="241">
       <c r="A241" s="1" t="n">
-        <v>669</v>
+        <v>239</v>
       </c>
       <c r="B241" t="n">
         <v>170491228</v>
@@ -13466,7 +13466,7 @@
     </row>
     <row r="242">
       <c r="A242" s="1" t="n">
-        <v>670</v>
+        <v>240</v>
       </c>
       <c r="B242" t="n">
         <v>170491229</v>
@@ -13512,7 +13512,7 @@
     </row>
     <row r="243">
       <c r="A243" s="1" t="n">
-        <v>672</v>
+        <v>241</v>
       </c>
       <c r="B243" t="n">
         <v>170491231</v>
@@ -13558,7 +13558,7 @@
     </row>
     <row r="244">
       <c r="A244" s="1" t="n">
-        <v>673</v>
+        <v>242</v>
       </c>
       <c r="B244" t="n">
         <v>170491232</v>
@@ -13604,7 +13604,7 @@
     </row>
     <row r="245">
       <c r="A245" s="1" t="n">
-        <v>698</v>
+        <v>243</v>
       </c>
       <c r="B245" t="n">
         <v>170652139</v>
@@ -13660,7 +13660,7 @@
     </row>
     <row r="246">
       <c r="A246" s="1" t="n">
-        <v>699</v>
+        <v>244</v>
       </c>
       <c r="B246" t="n">
         <v>170652143</v>
@@ -13716,7 +13716,7 @@
     </row>
     <row r="247">
       <c r="A247" s="1" t="n">
-        <v>704</v>
+        <v>245</v>
       </c>
       <c r="B247" t="n">
         <v>170652430</v>
@@ -13772,7 +13772,7 @@
     </row>
     <row r="248">
       <c r="A248" s="1" t="n">
-        <v>706</v>
+        <v>246</v>
       </c>
       <c r="B248" t="n">
         <v>170652432</v>
@@ -13828,7 +13828,7 @@
     </row>
     <row r="249">
       <c r="A249" s="1" t="n">
-        <v>708</v>
+        <v>247</v>
       </c>
       <c r="B249" t="n">
         <v>170652474</v>
@@ -13874,7 +13874,7 @@
     </row>
     <row r="250">
       <c r="A250" s="1" t="n">
-        <v>710</v>
+        <v>248</v>
       </c>
       <c r="B250" t="n">
         <v>170652878</v>
@@ -13930,7 +13930,7 @@
     </row>
     <row r="251">
       <c r="A251" s="1" t="n">
-        <v>719</v>
+        <v>249</v>
       </c>
       <c r="B251" t="n">
         <v>170841071</v>
@@ -13986,7 +13986,7 @@
     </row>
     <row r="252">
       <c r="A252" s="1" t="n">
-        <v>726</v>
+        <v>250</v>
       </c>
       <c r="B252" t="n">
         <v>171231062</v>
@@ -14032,7 +14032,7 @@
     </row>
     <row r="253">
       <c r="A253" s="1" t="n">
-        <v>727</v>
+        <v>251</v>
       </c>
       <c r="B253" t="n">
         <v>171231063</v>
@@ -14078,7 +14078,7 @@
     </row>
     <row r="254">
       <c r="A254" s="1" t="n">
-        <v>734</v>
+        <v>252</v>
       </c>
       <c r="B254" t="n">
         <v>172351131</v>
@@ -14134,7 +14134,7 @@
     </row>
     <row r="255">
       <c r="A255" s="1" t="n">
-        <v>735</v>
+        <v>253</v>
       </c>
       <c r="B255" t="n">
         <v>172351143</v>
@@ -14190,7 +14190,7 @@
     </row>
     <row r="256">
       <c r="A256" s="1" t="n">
-        <v>743</v>
+        <v>254</v>
       </c>
       <c r="B256" t="n">
         <v>172600583</v>
@@ -14236,7 +14236,7 @@
     </row>
     <row r="257">
       <c r="A257" s="1" t="n">
-        <v>744</v>
+        <v>255</v>
       </c>
       <c r="B257" t="n">
         <v>172600586</v>
@@ -14282,7 +14282,7 @@
     </row>
     <row r="258">
       <c r="A258" s="1" t="n">
-        <v>746</v>
+        <v>256</v>
       </c>
       <c r="B258" t="n">
         <v>172601000</v>
@@ -14328,7 +14328,7 @@
     </row>
     <row r="259">
       <c r="A259" s="1" t="n">
-        <v>748</v>
+        <v>257</v>
       </c>
       <c r="B259" t="n">
         <v>172601007</v>
@@ -14378,7 +14378,7 @@
     </row>
     <row r="260">
       <c r="A260" s="1" t="n">
-        <v>751</v>
+        <v>258</v>
       </c>
       <c r="B260" t="n">
         <v>172601017</v>
@@ -14424,7 +14424,7 @@
     </row>
     <row r="261">
       <c r="A261" s="1" t="n">
-        <v>752</v>
+        <v>259</v>
       </c>
       <c r="B261" t="n">
         <v>172601018</v>
@@ -14456,7 +14456,7 @@
         <v>-40</v>
       </c>
       <c r="O261" t="n">
-        <v>-7</v>
+        <v>54</v>
       </c>
       <c r="P261" t="n">
         <v>4488000</v>
@@ -14470,7 +14470,7 @@
     </row>
     <row r="262">
       <c r="A262" s="1" t="n">
-        <v>753</v>
+        <v>260</v>
       </c>
       <c r="B262" t="n">
         <v>172601019</v>
@@ -14516,7 +14516,7 @@
     </row>
     <row r="263">
       <c r="A263" s="1" t="n">
-        <v>760</v>
+        <v>261</v>
       </c>
       <c r="B263" t="n">
         <v>172620505</v>
@@ -14572,7 +14572,7 @@
     </row>
     <row r="264">
       <c r="A264" s="1" t="n">
-        <v>763</v>
+        <v>262</v>
       </c>
       <c r="B264" t="n">
         <v>172620527</v>
@@ -14628,7 +14628,7 @@
     </row>
     <row r="265">
       <c r="A265" s="1" t="n">
-        <v>764</v>
+        <v>263</v>
       </c>
       <c r="B265" t="n">
         <v>172620528</v>
@@ -14684,7 +14684,7 @@
     </row>
     <row r="266">
       <c r="A266" s="1" t="n">
-        <v>765</v>
+        <v>264</v>
       </c>
       <c r="B266" t="n">
         <v>172620529</v>
@@ -14740,7 +14740,7 @@
     </row>
     <row r="267">
       <c r="A267" s="1" t="n">
-        <v>766</v>
+        <v>265</v>
       </c>
       <c r="B267" t="n">
         <v>172620566</v>
@@ -14796,7 +14796,7 @@
     </row>
     <row r="268">
       <c r="A268" s="1" t="n">
-        <v>767</v>
+        <v>266</v>
       </c>
       <c r="B268" t="n">
         <v>172620572</v>
@@ -14838,7 +14838,7 @@
         <v>-53</v>
       </c>
       <c r="O268" t="n">
-        <v>-11</v>
+        <v>41</v>
       </c>
       <c r="P268" t="n">
         <v>7949200</v>
@@ -14852,7 +14852,7 @@
     </row>
     <row r="269">
       <c r="A269" s="1" t="n">
-        <v>771</v>
+        <v>267</v>
       </c>
       <c r="B269" t="n">
         <v>172620580</v>
@@ -14908,7 +14908,7 @@
     </row>
     <row r="270">
       <c r="A270" s="1" t="n">
-        <v>773</v>
+        <v>268</v>
       </c>
       <c r="B270" t="n">
         <v>172620583</v>
@@ -14964,7 +14964,7 @@
     </row>
     <row r="271">
       <c r="A271" s="1" t="n">
-        <v>775</v>
+        <v>269</v>
       </c>
       <c r="B271" t="n">
         <v>172620586</v>
@@ -15020,7 +15020,7 @@
     </row>
     <row r="272">
       <c r="A272" s="1" t="n">
-        <v>776</v>
+        <v>270</v>
       </c>
       <c r="B272" t="n">
         <v>172620587</v>
@@ -15076,7 +15076,7 @@
     </row>
     <row r="273">
       <c r="A273" s="1" t="n">
-        <v>780</v>
+        <v>271</v>
       </c>
       <c r="B273" t="n">
         <v>172620595</v>
@@ -15132,7 +15132,7 @@
     </row>
     <row r="274">
       <c r="A274" s="1" t="n">
-        <v>781</v>
+        <v>272</v>
       </c>
       <c r="B274" t="n">
         <v>172620596</v>
@@ -15188,7 +15188,7 @@
     </row>
     <row r="275">
       <c r="A275" s="1" t="n">
-        <v>783</v>
+        <v>273</v>
       </c>
       <c r="B275" t="n">
         <v>172620598</v>
@@ -15244,7 +15244,7 @@
     </row>
     <row r="276">
       <c r="A276" s="1" t="n">
-        <v>787</v>
+        <v>274</v>
       </c>
       <c r="B276" t="n">
         <v>172620603</v>
@@ -15286,7 +15286,7 @@
         <v>-46</v>
       </c>
       <c r="O276" t="n">
-        <v>-14</v>
+        <v>48</v>
       </c>
       <c r="P276" t="n">
         <v>4488000</v>
@@ -15300,7 +15300,7 @@
     </row>
     <row r="277">
       <c r="A277" s="1" t="n">
-        <v>788</v>
+        <v>275</v>
       </c>
       <c r="B277" t="n">
         <v>172620604</v>
@@ -15356,7 +15356,7 @@
     </row>
     <row r="278">
       <c r="A278" s="1" t="n">
-        <v>792</v>
+        <v>276</v>
       </c>
       <c r="B278" t="n">
         <v>172840052</v>
@@ -15402,7 +15402,7 @@
     </row>
     <row r="279">
       <c r="A279" s="1" t="n">
-        <v>794</v>
+        <v>277</v>
       </c>
       <c r="B279" t="n">
         <v>172870234</v>
@@ -15434,7 +15434,7 @@
         <v>-54</v>
       </c>
       <c r="O279" t="n">
-        <v>-10</v>
+        <v>40</v>
       </c>
       <c r="P279" t="n">
         <v>8884600</v>
@@ -15448,7 +15448,7 @@
     </row>
     <row r="280">
       <c r="A280" s="1" t="n">
-        <v>795</v>
+        <v>278</v>
       </c>
       <c r="B280" t="n">
         <v>172870235</v>
@@ -15480,7 +15480,7 @@
         <v>-54</v>
       </c>
       <c r="O280" t="n">
-        <v>-9</v>
+        <v>40</v>
       </c>
       <c r="P280" t="n">
         <v>8680000</v>
@@ -15494,7 +15494,7 @@
     </row>
     <row r="281">
       <c r="A281" s="1" t="n">
-        <v>796</v>
+        <v>279</v>
       </c>
       <c r="B281" t="n">
         <v>172870236</v>
@@ -15540,7 +15540,7 @@
     </row>
     <row r="282">
       <c r="A282" s="1" t="n">
-        <v>798</v>
+        <v>280</v>
       </c>
       <c r="B282" t="n">
         <v>172870240</v>
@@ -15586,7 +15586,7 @@
     </row>
     <row r="283">
       <c r="A283" s="1" t="n">
-        <v>809</v>
+        <v>281</v>
       </c>
       <c r="B283" t="n">
         <v>173040866</v>
@@ -15642,7 +15642,7 @@
     </row>
     <row r="284">
       <c r="A284" s="1" t="n">
-        <v>815</v>
+        <v>282</v>
       </c>
       <c r="B284" t="n">
         <v>173041070</v>
@@ -15698,7 +15698,7 @@
     </row>
     <row r="285">
       <c r="A285" s="1" t="n">
-        <v>816</v>
+        <v>283</v>
       </c>
       <c r="B285" t="n">
         <v>173041071</v>
@@ -15754,7 +15754,7 @@
     </row>
     <row r="286">
       <c r="A286" s="1" t="n">
-        <v>817</v>
+        <v>284</v>
       </c>
       <c r="B286" t="n">
         <v>173041072</v>
@@ -15810,7 +15810,7 @@
     </row>
     <row r="287">
       <c r="A287" s="1" t="n">
-        <v>819</v>
+        <v>285</v>
       </c>
       <c r="B287" t="n">
         <v>173041074</v>
@@ -15866,7 +15866,7 @@
     </row>
     <row r="288">
       <c r="A288" s="1" t="n">
-        <v>821</v>
+        <v>286</v>
       </c>
       <c r="B288" t="n">
         <v>173041076</v>
@@ -15922,7 +15922,7 @@
     </row>
     <row r="289">
       <c r="A289" s="1" t="n">
-        <v>822</v>
+        <v>287</v>
       </c>
       <c r="B289" t="n">
         <v>173041077</v>
@@ -15978,7 +15978,7 @@
     </row>
     <row r="290">
       <c r="A290" s="1" t="n">
-        <v>823</v>
+        <v>288</v>
       </c>
       <c r="B290" t="n">
         <v>173041078</v>
@@ -16034,7 +16034,7 @@
     </row>
     <row r="291">
       <c r="A291" s="1" t="n">
-        <v>825</v>
+        <v>289</v>
       </c>
       <c r="B291" t="n">
         <v>173041081</v>
@@ -16090,7 +16090,7 @@
     </row>
     <row r="292">
       <c r="A292" s="1" t="n">
-        <v>831</v>
+        <v>290</v>
       </c>
       <c r="B292" t="n">
         <v>173041087</v>
@@ -16146,7 +16146,7 @@
     </row>
     <row r="293">
       <c r="A293" s="1" t="n">
-        <v>832</v>
+        <v>291</v>
       </c>
       <c r="B293" t="n">
         <v>173041088</v>
@@ -16202,7 +16202,7 @@
     </row>
     <row r="294">
       <c r="A294" s="1" t="n">
-        <v>833</v>
+        <v>292</v>
       </c>
       <c r="B294" t="n">
         <v>173041091</v>
@@ -16258,7 +16258,7 @@
     </row>
     <row r="295">
       <c r="A295" s="1" t="n">
-        <v>834</v>
+        <v>293</v>
       </c>
       <c r="B295" t="n">
         <v>173041092</v>
@@ -16314,7 +16314,7 @@
     </row>
     <row r="296">
       <c r="A296" s="1" t="n">
-        <v>838</v>
+        <v>294</v>
       </c>
       <c r="B296" t="n">
         <v>173041097</v>
@@ -16370,7 +16370,7 @@
     </row>
     <row r="297">
       <c r="A297" s="1" t="n">
-        <v>839</v>
+        <v>295</v>
       </c>
       <c r="B297" t="n">
         <v>173041098</v>
@@ -16426,7 +16426,7 @@
     </row>
     <row r="298">
       <c r="A298" s="1" t="n">
-        <v>840</v>
+        <v>296</v>
       </c>
       <c r="B298" t="n">
         <v>173041099</v>
@@ -16482,7 +16482,7 @@
     </row>
     <row r="299">
       <c r="A299" s="1" t="n">
-        <v>843</v>
+        <v>297</v>
       </c>
       <c r="B299" t="n">
         <v>173041302</v>
@@ -16524,7 +16524,7 @@
         <v>-60</v>
       </c>
       <c r="O299" t="n">
-        <v>-4</v>
+        <v>34</v>
       </c>
       <c r="P299" t="n">
         <v>392000</v>
@@ -16538,7 +16538,7 @@
     </row>
     <row r="300">
       <c r="A300" s="1" t="n">
-        <v>844</v>
+        <v>298</v>
       </c>
       <c r="B300" t="n">
         <v>173041307</v>
@@ -16594,7 +16594,7 @@
     </row>
     <row r="301">
       <c r="A301" s="1" t="n">
-        <v>845</v>
+        <v>299</v>
       </c>
       <c r="B301" t="n">
         <v>173041308</v>
@@ -16650,7 +16650,7 @@
     </row>
     <row r="302">
       <c r="A302" s="1" t="n">
-        <v>846</v>
+        <v>300</v>
       </c>
       <c r="B302" t="n">
         <v>173041309</v>
@@ -16706,7 +16706,7 @@
     </row>
     <row r="303">
       <c r="A303" s="1" t="n">
-        <v>847</v>
+        <v>301</v>
       </c>
       <c r="B303" t="n">
         <v>173041310</v>
@@ -16762,7 +16762,7 @@
     </row>
     <row r="304">
       <c r="A304" s="1" t="n">
-        <v>848</v>
+        <v>302</v>
       </c>
       <c r="B304" t="n">
         <v>173041311</v>
@@ -16818,7 +16818,7 @@
     </row>
     <row r="305">
       <c r="A305" s="1" t="n">
-        <v>849</v>
+        <v>303</v>
       </c>
       <c r="B305" t="n">
         <v>173041312</v>
@@ -16874,7 +16874,7 @@
     </row>
     <row r="306">
       <c r="A306" s="1" t="n">
-        <v>850</v>
+        <v>304</v>
       </c>
       <c r="B306" t="n">
         <v>173041313</v>
@@ -16916,7 +16916,7 @@
         <v>-25</v>
       </c>
       <c r="O306" t="n">
-        <v>-13</v>
+        <v>69</v>
       </c>
       <c r="P306" t="n">
         <v>529200</v>
@@ -16930,7 +16930,7 @@
     </row>
     <row r="307">
       <c r="A307" s="1" t="n">
-        <v>851</v>
+        <v>305</v>
       </c>
       <c r="B307" t="n">
         <v>173041317</v>
@@ -16986,7 +16986,7 @@
     </row>
     <row r="308">
       <c r="A308" s="1" t="n">
-        <v>853</v>
+        <v>306</v>
       </c>
       <c r="B308" t="n">
         <v>173041319</v>
@@ -17042,7 +17042,7 @@
     </row>
     <row r="309">
       <c r="A309" s="1" t="n">
-        <v>856</v>
+        <v>307</v>
       </c>
       <c r="B309" t="n">
         <v>173041340</v>
@@ -17098,7 +17098,7 @@
     </row>
     <row r="310">
       <c r="A310" s="1" t="n">
-        <v>858</v>
+        <v>308</v>
       </c>
       <c r="B310" t="n">
         <v>173041357</v>
@@ -17154,7 +17154,7 @@
     </row>
     <row r="311">
       <c r="A311" s="1" t="n">
-        <v>859</v>
+        <v>309</v>
       </c>
       <c r="B311" t="n">
         <v>173041358</v>
@@ -17210,7 +17210,7 @@
     </row>
     <row r="312">
       <c r="A312" s="1" t="n">
-        <v>862</v>
+        <v>310</v>
       </c>
       <c r="B312" t="n">
         <v>173041386</v>
@@ -17252,7 +17252,7 @@
         <v>-58</v>
       </c>
       <c r="O312" t="n">
-        <v>-2</v>
+        <v>36</v>
       </c>
       <c r="P312" t="n">
         <v>1061200</v>
@@ -17266,7 +17266,7 @@
     </row>
     <row r="313">
       <c r="A313" s="1" t="n">
-        <v>863</v>
+        <v>311</v>
       </c>
       <c r="B313" t="n">
         <v>173041400</v>
@@ -17322,7 +17322,7 @@
     </row>
     <row r="314">
       <c r="A314" s="1" t="n">
-        <v>866</v>
+        <v>312</v>
       </c>
       <c r="B314" t="n">
         <v>173041800</v>
@@ -17378,7 +17378,7 @@
     </row>
     <row r="315">
       <c r="A315" s="1" t="n">
-        <v>868</v>
+        <v>313</v>
       </c>
       <c r="B315" t="n">
         <v>173041802</v>
@@ -17434,7 +17434,7 @@
     </row>
     <row r="316">
       <c r="A316" s="1" t="n">
-        <v>870</v>
+        <v>314</v>
       </c>
       <c r="B316" t="n">
         <v>173041804</v>
@@ -17480,7 +17480,7 @@
     </row>
     <row r="317">
       <c r="A317" s="1" t="n">
-        <v>871</v>
+        <v>315</v>
       </c>
       <c r="B317" t="n">
         <v>173041805</v>
@@ -17526,7 +17526,7 @@
     </row>
     <row r="318">
       <c r="A318" s="1" t="n">
-        <v>872</v>
+        <v>316</v>
       </c>
       <c r="B318" t="n">
         <v>173041806</v>
@@ -17572,7 +17572,7 @@
     </row>
     <row r="319">
       <c r="A319" s="1" t="n">
-        <v>873</v>
+        <v>317</v>
       </c>
       <c r="B319" t="n">
         <v>173041807</v>
@@ -17618,7 +17618,7 @@
     </row>
     <row r="320">
       <c r="A320" s="1" t="n">
-        <v>874</v>
+        <v>318</v>
       </c>
       <c r="B320" t="n">
         <v>173041808</v>
@@ -17664,7 +17664,7 @@
     </row>
     <row r="321">
       <c r="A321" s="1" t="n">
-        <v>881</v>
+        <v>319</v>
       </c>
       <c r="B321" t="n">
         <v>173050542</v>
@@ -17696,7 +17696,7 @@
         <v>-3</v>
       </c>
       <c r="O321" t="n">
-        <v>-35</v>
+        <v>91</v>
       </c>
       <c r="P321" t="n">
         <v>56000</v>
@@ -17710,7 +17710,7 @@
     </row>
     <row r="322">
       <c r="A322" s="1" t="n">
-        <v>885</v>
+        <v>320</v>
       </c>
       <c r="B322" t="n">
         <v>173050549</v>
@@ -17756,7 +17756,7 @@
     </row>
     <row r="323">
       <c r="A323" s="1" t="n">
-        <v>886</v>
+        <v>321</v>
       </c>
       <c r="B323" t="n">
         <v>173050550</v>
@@ -17802,7 +17802,7 @@
     </row>
     <row r="324">
       <c r="A324" s="1" t="n">
-        <v>888</v>
+        <v>322</v>
       </c>
       <c r="B324" t="n">
         <v>173050552</v>
@@ -17848,7 +17848,7 @@
     </row>
     <row r="325">
       <c r="A325" s="1" t="n">
-        <v>889</v>
+        <v>323</v>
       </c>
       <c r="B325" t="n">
         <v>173050553</v>
@@ -17894,7 +17894,7 @@
     </row>
     <row r="326">
       <c r="A326" s="1" t="n">
-        <v>892</v>
+        <v>324</v>
       </c>
       <c r="B326" t="n">
         <v>173050652</v>
@@ -17926,7 +17926,7 @@
         <v>-60</v>
       </c>
       <c r="O326" t="n">
-        <v>-4</v>
+        <v>34</v>
       </c>
       <c r="P326" t="n">
         <v>10098000</v>
@@ -17940,7 +17940,7 @@
     </row>
     <row r="327">
       <c r="A327" s="1" t="n">
-        <v>893</v>
+        <v>325</v>
       </c>
       <c r="B327" t="n">
         <v>173050654</v>
@@ -17986,7 +17986,7 @@
     </row>
     <row r="328">
       <c r="A328" s="1" t="n">
-        <v>894</v>
+        <v>326</v>
       </c>
       <c r="B328" t="n">
         <v>173050655</v>
@@ -18032,7 +18032,7 @@
     </row>
     <row r="329">
       <c r="A329" s="1" t="n">
-        <v>896</v>
+        <v>327</v>
       </c>
       <c r="B329" t="n">
         <v>173050661</v>
@@ -18076,7 +18076,7 @@
     </row>
     <row r="330">
       <c r="A330" s="1" t="n">
-        <v>897</v>
+        <v>328</v>
       </c>
       <c r="B330" t="n">
         <v>173050666</v>
@@ -18120,7 +18120,7 @@
     </row>
     <row r="331">
       <c r="A331" s="1" t="n">
-        <v>898</v>
+        <v>329</v>
       </c>
       <c r="B331" t="n">
         <v>173050668</v>
@@ -18166,7 +18166,7 @@
     </row>
     <row r="332">
       <c r="A332" s="1" t="n">
-        <v>901</v>
+        <v>330</v>
       </c>
       <c r="B332" t="n">
         <v>173050672</v>
@@ -18212,7 +18212,7 @@
     </row>
     <row r="333">
       <c r="A333" s="1" t="n">
-        <v>903</v>
+        <v>331</v>
       </c>
       <c r="B333" t="n">
         <v>173050674</v>
@@ -18258,7 +18258,7 @@
     </row>
     <row r="334">
       <c r="A334" s="1" t="n">
-        <v>904</v>
+        <v>332</v>
       </c>
       <c r="B334" t="n">
         <v>173050675</v>
@@ -18302,7 +18302,7 @@
     </row>
     <row r="335">
       <c r="A335" s="1" t="n">
-        <v>914</v>
+        <v>333</v>
       </c>
       <c r="B335" t="n">
         <v>173051001</v>
@@ -18358,7 +18358,7 @@
     </row>
     <row r="336">
       <c r="A336" s="1" t="n">
-        <v>919</v>
+        <v>334</v>
       </c>
       <c r="B336" t="n">
         <v>173051006</v>
@@ -18414,7 +18414,7 @@
     </row>
     <row r="337">
       <c r="A337" s="1" t="n">
-        <v>920</v>
+        <v>335</v>
       </c>
       <c r="B337" t="n">
         <v>173051008</v>
@@ -18470,7 +18470,7 @@
     </row>
     <row r="338">
       <c r="A338" s="1" t="n">
-        <v>921</v>
+        <v>336</v>
       </c>
       <c r="B338" t="n">
         <v>173051009</v>
@@ -18516,7 +18516,7 @@
     </row>
     <row r="339">
       <c r="A339" s="1" t="n">
-        <v>926</v>
+        <v>337</v>
       </c>
       <c r="B339" t="n">
         <v>173051016</v>
@@ -18558,7 +18558,7 @@
         <v>-61</v>
       </c>
       <c r="O339" t="n">
-        <v>-3</v>
+        <v>33</v>
       </c>
       <c r="P339" t="n">
         <v>26935000</v>
@@ -18572,7 +18572,7 @@
     </row>
     <row r="340">
       <c r="A340" s="1" t="n">
-        <v>934</v>
+        <v>338</v>
       </c>
       <c r="B340" t="n">
         <v>173240133</v>
@@ -18628,7 +18628,7 @@
     </row>
     <row r="341">
       <c r="A341" s="1" t="n">
-        <v>935</v>
+        <v>339</v>
       </c>
       <c r="B341" t="n">
         <v>173240136</v>
@@ -18684,7 +18684,7 @@
     </row>
     <row r="342">
       <c r="A342" s="1" t="n">
-        <v>943</v>
+        <v>340</v>
       </c>
       <c r="B342" t="n">
         <v>173240302</v>
@@ -18740,7 +18740,7 @@
     </row>
     <row r="343">
       <c r="A343" s="1" t="n">
-        <v>946</v>
+        <v>341</v>
       </c>
       <c r="B343" t="n">
         <v>173240339</v>
@@ -18782,7 +18782,7 @@
         <v>108</v>
       </c>
       <c r="O343" t="n">
-        <v>-1</v>
+        <v>202</v>
       </c>
       <c r="P343" t="n">
         <v>784000</v>
@@ -18796,7 +18796,7 @@
     </row>
     <row r="344">
       <c r="A344" s="1" t="n">
-        <v>947</v>
+        <v>342</v>
       </c>
       <c r="B344" t="n">
         <v>173240405</v>
@@ -18852,7 +18852,7 @@
     </row>
     <row r="345">
       <c r="A345" s="1" t="n">
-        <v>948</v>
+        <v>343</v>
       </c>
       <c r="B345" t="n">
         <v>173240406</v>
@@ -18908,7 +18908,7 @@
     </row>
     <row r="346">
       <c r="A346" s="1" t="n">
-        <v>949</v>
+        <v>344</v>
       </c>
       <c r="B346" t="n">
         <v>173240408</v>
@@ -18964,7 +18964,7 @@
     </row>
     <row r="347">
       <c r="A347" s="1" t="n">
-        <v>952</v>
+        <v>345</v>
       </c>
       <c r="B347" t="n">
         <v>173301002</v>
@@ -19020,7 +19020,7 @@
     </row>
     <row r="348">
       <c r="A348" s="1" t="n">
-        <v>953</v>
+        <v>346</v>
       </c>
       <c r="B348" t="n">
         <v>173301003</v>
@@ -19076,7 +19076,7 @@
     </row>
     <row r="349">
       <c r="A349" s="1" t="n">
-        <v>954</v>
+        <v>347</v>
       </c>
       <c r="B349" t="n">
         <v>173301004</v>
@@ -19126,7 +19126,7 @@
     </row>
     <row r="350">
       <c r="A350" s="1" t="n">
-        <v>955</v>
+        <v>348</v>
       </c>
       <c r="B350" t="n">
         <v>173301005</v>
@@ -19182,7 +19182,7 @@
     </row>
     <row r="351">
       <c r="A351" s="1" t="n">
-        <v>956</v>
+        <v>349</v>
       </c>
       <c r="B351" t="n">
         <v>173301006</v>
@@ -19238,7 +19238,7 @@
     </row>
     <row r="352">
       <c r="A352" s="1" t="n">
-        <v>960</v>
+        <v>350</v>
       </c>
       <c r="B352" t="n">
         <v>173400203</v>
@@ -19294,7 +19294,7 @@
     </row>
     <row r="353">
       <c r="A353" s="1" t="n">
-        <v>961</v>
+        <v>351</v>
       </c>
       <c r="B353" t="n">
         <v>173430131</v>
@@ -19350,7 +19350,7 @@
     </row>
     <row r="354">
       <c r="A354" s="1" t="n">
-        <v>962</v>
+        <v>352</v>
       </c>
       <c r="B354" t="n">
         <v>173430205</v>
@@ -19392,7 +19392,7 @@
         <v>53</v>
       </c>
       <c r="O354" t="n">
-        <v>-20</v>
+        <v>147</v>
       </c>
       <c r="P354" t="n">
         <v>810000</v>
@@ -19406,7 +19406,7 @@
     </row>
     <row r="355">
       <c r="A355" s="1" t="n">
-        <v>963</v>
+        <v>353</v>
       </c>
       <c r="B355" t="n">
         <v>173480103</v>
@@ -19448,7 +19448,7 @@
         <v>-53</v>
       </c>
       <c r="O355" t="n">
-        <v>-9</v>
+        <v>41</v>
       </c>
       <c r="P355" t="n">
         <v>893200</v>
@@ -19462,7 +19462,7 @@
     </row>
     <row r="356">
       <c r="A356" s="1" t="n">
-        <v>964</v>
+        <v>354</v>
       </c>
       <c r="B356" t="n">
         <v>173480106</v>
@@ -19518,7 +19518,7 @@
     </row>
     <row r="357">
       <c r="A357" s="1" t="n">
-        <v>965</v>
+        <v>355</v>
       </c>
       <c r="B357" t="n">
         <v>174020102</v>
@@ -19574,7 +19574,7 @@
     </row>
     <row r="358">
       <c r="A358" s="1" t="n">
-        <v>967</v>
+        <v>356</v>
       </c>
       <c r="B358" t="n">
         <v>174020108</v>
@@ -19630,7 +19630,7 @@
     </row>
     <row r="359">
       <c r="A359" s="1" t="n">
-        <v>968</v>
+        <v>357</v>
       </c>
       <c r="B359" t="n">
         <v>174020112</v>
@@ -19686,7 +19686,7 @@
     </row>
     <row r="360">
       <c r="A360" s="1" t="n">
-        <v>969</v>
+        <v>358</v>
       </c>
       <c r="B360" t="n">
         <v>174020115</v>
@@ -19742,7 +19742,7 @@
     </row>
     <row r="361">
       <c r="A361" s="1" t="n">
-        <v>976</v>
+        <v>359</v>
       </c>
       <c r="B361" t="n">
         <v>182010122</v>
@@ -19798,7 +19798,7 @@
     </row>
     <row r="362">
       <c r="A362" s="1" t="n">
-        <v>977</v>
+        <v>360</v>
       </c>
       <c r="B362" t="n">
         <v>182040102</v>
@@ -19854,7 +19854,7 @@
     </row>
     <row r="363">
       <c r="A363" s="1" t="n">
-        <v>979</v>
+        <v>361</v>
       </c>
       <c r="B363" t="n">
         <v>182040114</v>
@@ -19896,7 +19896,7 @@
         <v>-59</v>
       </c>
       <c r="O363" t="n">
-        <v>-5</v>
+        <v>35</v>
       </c>
       <c r="P363" t="n">
         <v>448000</v>
@@ -19910,7 +19910,7 @@
     </row>
     <row r="364">
       <c r="A364" s="1" t="n">
-        <v>980</v>
+        <v>362</v>
       </c>
       <c r="B364" t="n">
         <v>182040121</v>
@@ -19966,7 +19966,7 @@
     </row>
     <row r="365">
       <c r="A365" s="1" t="n">
-        <v>982</v>
+        <v>363</v>
       </c>
       <c r="B365" t="n">
         <v>182040131</v>
@@ -20022,7 +20022,7 @@
     </row>
     <row r="366">
       <c r="A366" s="1" t="n">
-        <v>983</v>
+        <v>364</v>
       </c>
       <c r="B366" t="n">
         <v>182040132</v>
@@ -20035,7 +20035,9 @@
       <c r="H366" t="inlineStr"/>
       <c r="I366" t="inlineStr"/>
       <c r="J366" t="inlineStr"/>
-      <c r="K366" t="inlineStr"/>
+      <c r="K366" s="2" t="n">
+        <v>44562</v>
+      </c>
       <c r="L366" t="inlineStr"/>
       <c r="M366" s="2" t="n">
         <v>44915</v>
@@ -20056,7 +20058,7 @@
     </row>
     <row r="367">
       <c r="A367" s="1" t="n">
-        <v>986</v>
+        <v>365</v>
       </c>
       <c r="B367" t="n">
         <v>182080220</v>
@@ -20112,7 +20114,7 @@
     </row>
     <row r="368">
       <c r="A368" s="1" t="n">
-        <v>988</v>
+        <v>366</v>
       </c>
       <c r="B368" t="n">
         <v>182080224</v>
@@ -20168,7 +20170,7 @@
     </row>
     <row r="369">
       <c r="A369" s="1" t="n">
-        <v>990</v>
+        <v>367</v>
       </c>
       <c r="B369" t="n">
         <v>182080227</v>
@@ -20224,7 +20226,7 @@
     </row>
     <row r="370">
       <c r="A370" s="1" t="n">
-        <v>991</v>
+        <v>368</v>
       </c>
       <c r="B370" t="n">
         <v>182080229</v>
@@ -20280,7 +20282,7 @@
     </row>
     <row r="371">
       <c r="A371" s="1" t="n">
-        <v>993</v>
+        <v>369</v>
       </c>
       <c r="B371" t="n">
         <v>182080232</v>
@@ -20336,7 +20338,7 @@
     </row>
     <row r="372">
       <c r="A372" s="1" t="n">
-        <v>994</v>
+        <v>370</v>
       </c>
       <c r="B372" t="n">
         <v>182080234</v>
@@ -20368,7 +20370,7 @@
         <v>9</v>
       </c>
       <c r="O372" t="n">
-        <v>-49</v>
+        <v>103</v>
       </c>
       <c r="P372" t="n">
         <v>19200</v>
@@ -20382,7 +20384,7 @@
     </row>
     <row r="373">
       <c r="A373" s="1" t="n">
-        <v>998</v>
+        <v>371</v>
       </c>
       <c r="B373" t="n">
         <v>182080240</v>
@@ -20438,7 +20440,7 @@
     </row>
     <row r="374">
       <c r="A374" s="1" t="n">
-        <v>999</v>
+        <v>372</v>
       </c>
       <c r="B374" t="n">
         <v>182080241</v>
@@ -20494,7 +20496,7 @@
     </row>
     <row r="375">
       <c r="A375" s="1" t="n">
-        <v>1000</v>
+        <v>373</v>
       </c>
       <c r="B375" t="n">
         <v>182080242</v>
@@ -20550,7 +20552,7 @@
     </row>
     <row r="376">
       <c r="A376" s="1" t="n">
-        <v>1001</v>
+        <v>374</v>
       </c>
       <c r="B376" t="n">
         <v>182080243</v>
@@ -20606,7 +20608,7 @@
     </row>
     <row r="377">
       <c r="A377" s="1" t="n">
-        <v>1004</v>
+        <v>375</v>
       </c>
       <c r="B377" t="n">
         <v>182080247</v>
@@ -20662,7 +20664,7 @@
     </row>
     <row r="378">
       <c r="A378" s="1" t="n">
-        <v>1007</v>
+        <v>376</v>
       </c>
       <c r="B378" t="n">
         <v>182080254</v>
@@ -20718,7 +20720,7 @@
     </row>
     <row r="379">
       <c r="A379" s="1" t="n">
-        <v>1008</v>
+        <v>377</v>
       </c>
       <c r="B379" t="n">
         <v>182080255</v>
@@ -20774,7 +20776,7 @@
     </row>
     <row r="380">
       <c r="A380" s="1" t="n">
-        <v>1010</v>
+        <v>378</v>
       </c>
       <c r="B380" t="n">
         <v>182080257</v>
@@ -20830,7 +20832,7 @@
     </row>
     <row r="381">
       <c r="A381" s="1" t="n">
-        <v>1011</v>
+        <v>379</v>
       </c>
       <c r="B381" t="n">
         <v>182080258</v>
@@ -20876,7 +20878,7 @@
     </row>
     <row r="382">
       <c r="A382" s="1" t="n">
-        <v>1012</v>
+        <v>380</v>
       </c>
       <c r="B382" t="n">
         <v>182080259</v>
@@ -20932,7 +20934,7 @@
     </row>
     <row r="383">
       <c r="A383" s="1" t="n">
-        <v>1013</v>
+        <v>381</v>
       </c>
       <c r="B383" t="n">
         <v>182080260</v>
@@ -20988,7 +20990,7 @@
     </row>
     <row r="384">
       <c r="A384" s="1" t="n">
-        <v>1014</v>
+        <v>382</v>
       </c>
       <c r="B384" t="n">
         <v>182130161</v>

</xml_diff>